<commit_message>
update with second semester
</commit_message>
<xml_diff>
--- a/Documents/Test case.xlsx
+++ b/Documents/Test case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexp\Desktop\HW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexp\Desktop\Code\School\sem2-2\tsh-2\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8855816E-47F6-40D0-966D-4D9571E64918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7469253A-4DEE-484E-A9D3-DF5A3F004355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="144">
   <si>
     <t>ID</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Admins and Customers can log out of the system</t>
   </si>
   <si>
-    <t>The user enters home page</t>
-  </si>
-  <si>
     <t>The user is shown log in page</t>
   </si>
   <si>
@@ -330,13 +327,151 @@
   </si>
   <si>
     <t>Using a browser's lighthouse test is indicating a percentage above 80</t>
+  </si>
+  <si>
+    <t>UC-17</t>
+  </si>
+  <si>
+    <t>UC-18</t>
+  </si>
+  <si>
+    <t>UC-19</t>
+  </si>
+  <si>
+    <t>TC-21</t>
+  </si>
+  <si>
+    <t>TC-22</t>
+  </si>
+  <si>
+    <t>TC-23</t>
+  </si>
+  <si>
+    <t>UC-20</t>
+  </si>
+  <si>
+    <t>TC-24</t>
+  </si>
+  <si>
+    <t>Web application is installable</t>
+  </si>
+  <si>
+    <t>Students can make event suggestions</t>
+  </si>
+  <si>
+    <t>Event organizer can accept event suggestion</t>
+  </si>
+  <si>
+    <t>Event organizer can broadcast messages</t>
+  </si>
+  <si>
+    <t>Lorem ipsum</t>
+  </si>
+  <si>
+    <t>All students in the same branch receive this notification</t>
+  </si>
+  <si>
+    <t>The event is made available for other students</t>
+  </si>
+  <si>
+    <t>Event organizer recieves notification and can accept or deny the suggestion</t>
+  </si>
+  <si>
+    <t>PWA is installed on the user's device</t>
+  </si>
+  <si>
+    <t>User must be logged in</t>
+  </si>
+  <si>
+    <t>User is logged in as event organizer and there is at least one suggestion</t>
+  </si>
+  <si>
+    <t>student@email student</t>
+  </si>
+  <si>
+    <t>student.comitee@email studentcomitee</t>
+  </si>
+  <si>
+    <t>event.organizer@email eventorganizer</t>
+  </si>
+  <si>
+    <t>admin@email admin</t>
+  </si>
+  <si>
+    <t>The user enters home page as admin</t>
+  </si>
+  <si>
+    <t>The user enters home page as student</t>
+  </si>
+  <si>
+    <t>The user enters home page as student on the comitee</t>
+  </si>
+  <si>
+    <t>The user enters home page as event organizer</t>
+  </si>
+  <si>
+    <t>123@email 123</t>
+  </si>
+  <si>
+    <t>The user is prompted to input a valid name</t>
+  </si>
+  <si>
+    <t>The user is prompted to input correct credentails</t>
+  </si>
+  <si>
+    <t>&lt;empty&gt;</t>
+  </si>
+  <si>
+    <t>The user is prompted to input valid data</t>
+  </si>
+  <si>
+    <t>Eindhoven,, student ,email, stansilav</t>
+  </si>
+  <si>
+    <t>User must be logged in as student, the event must be fully booked</t>
+  </si>
+  <si>
+    <t>To the student is explained that the event is fully booked and cannot join</t>
+  </si>
+  <si>
+    <t>TC-25</t>
+  </si>
+  <si>
+    <t>TC-26</t>
+  </si>
+  <si>
+    <t>TC-27</t>
+  </si>
+  <si>
+    <t>TC-28</t>
+  </si>
+  <si>
+    <t>TC-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The device supports pwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The device does not support pwa</t>
+  </si>
+  <si>
+    <t>PWA is not installed on the user's device</t>
+  </si>
+  <si>
+    <t>Party, A TSH PARTY!!, tsh</t>
+  </si>
+  <si>
+    <t>,,,</t>
+  </si>
+  <si>
+    <t>TC-30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +507,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -381,7 +531,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -456,11 +606,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -492,8 +676,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -584,8 +781,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FBA2B6B-7BEE-4EA9-A7BD-78B8B831E27F}" name="Table1" displayName="Table1" ref="C4:I20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="C4:I20" xr:uid="{2FBA2B6B-7BEE-4EA9-A7BD-78B8B831E27F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2FBA2B6B-7BEE-4EA9-A7BD-78B8B831E27F}" name="Table1" displayName="Table1" ref="C4:I34" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="C4:I34" xr:uid="{2FBA2B6B-7BEE-4EA9-A7BD-78B8B831E27F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{90DCBD7A-CF3A-4C56-9B5A-13390F0FB0DA}" name="ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{420A63C2-6FD5-4493-9043-1C1805CB8DC3}" name="UC" dataDxfId="5"/>
@@ -896,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:J25"/>
+  <dimension ref="C3:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,7 +1104,7 @@
     <col min="1" max="4" width="8.88671875" style="5"/>
     <col min="5" max="5" width="50.77734375" style="5" customWidth="1"/>
     <col min="6" max="6" width="24.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="40.21875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="51.77734375" style="5" customWidth="1"/>
     <col min="8" max="8" width="39" style="5" customWidth="1"/>
     <col min="9" max="9" width="39.109375" style="5" customWidth="1"/>
     <col min="10" max="10" width="42.5546875" style="5" customWidth="1"/>
@@ -947,7 +1144,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="3:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" ht="36" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -958,28 +1155,30 @@
         <v>23</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="H5" s="2" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="3:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" ht="36" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="H6" s="2" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -988,80 +1187,74 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="3:10" ht="36" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="3:10" ht="36" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="13" t="s">
+        <v>125</v>
+      </c>
       <c r="H9" s="2" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="3:10" ht="36" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="I10" s="4"/>
     </row>
@@ -1070,19 +1263,19 @@
         <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="I11" s="4"/>
     </row>
@@ -1091,250 +1284,539 @@
         <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="H12" s="2" t="s">
-        <v>41</v>
+        <v>126</v>
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="3:10" ht="54" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" ht="36" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="3:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="3:10" ht="54" x14ac:dyDescent="0.3">
-      <c r="C14" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="3:10" ht="36" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="3:10" ht="36" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="3:9" ht="54" x14ac:dyDescent="0.3">
-      <c r="C17" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="3:9" ht="36" x14ac:dyDescent="0.3">
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="H18" s="2" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="3:9" ht="36" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="3:9" ht="54" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="22" spans="3:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="C22" s="7" t="s">
+      <c r="D21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="3:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="C24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="3:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="C26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="3:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="C28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C30" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="3:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="C31" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C32" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="3:9" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C34" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="37" spans="3:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="C37" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="E37" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="3:9" ht="36" x14ac:dyDescent="0.3">
-      <c r="C23" s="7" t="s">
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C38" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="E38" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="3:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="C39" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="3:9" ht="54" x14ac:dyDescent="0.3">
-      <c r="C24" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="10" t="s">
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="3:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="C40" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8" t="s">
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="3:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="C25" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I25" s="9"/>
+      <c r="I40" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1" xr:uid="{01DD4813-DA1F-4FFC-8494-8A02E8EF187C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>